<commit_message>
0614 update CFT list
</commit_message>
<xml_diff>
--- a/GMLA loading analysis/PMsystem_PRweb/(Output) Projects (include ASIA SKU) in PM system without DPQE.xlsx
+++ b/GMLA loading analysis/PMsystem_PRweb/(Output) Projects (include ASIA SKU) in PM system without DPQE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Project Name</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>Honda MLJX RFQ</t>
-  </si>
-  <si>
-    <t>Instinct 2X Solar</t>
   </si>
   <si>
     <t>Asia</t>
@@ -429,7 +426,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -478,13 +475,13 @@
         <v>44774</v>
       </c>
       <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -498,13 +495,13 @@
         <v>46022</v>
       </c>
       <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
         <v>14</v>
       </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -518,38 +515,12 @@
         <v>45535</v>
       </c>
       <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
         <v>14</v>
       </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
       <c r="I4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1">
-        <v>16370</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2">
-        <v>44907</v>
-      </c>
-      <c r="E5" s="2">
-        <v>45012</v>
-      </c>
-      <c r="F5" s="2">
-        <v>44971</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>